<commit_message>
task responsibilities updated june
</commit_message>
<xml_diff>
--- a/tasks responsabilities.xlsx
+++ b/tasks responsabilities.xlsx
@@ -72,10 +72,10 @@
     <t xml:space="preserve">Third phase coding and testing </t>
   </si>
   <si>
-    <t xml:space="preserve">on going </t>
-  </si>
-  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Forth Phase for softwae and coding</t>
   </si>
 </sst>
 </file>
@@ -176,21 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -213,8 +201,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,7 +510,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,59 +526,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>19</v>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="3">
         <v>45027</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="7">
+      <c r="D3" s="3">
         <v>45027</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="7">
-        <v>45027</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="F3" s="3">
+        <v>45027</v>
+      </c>
+      <c r="G3" s="3">
         <v>45022</v>
       </c>
     </row>
@@ -589,18 +586,18 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="3">
         <v>45027</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="7">
+      <c r="D4" s="3">
         <v>45027</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="7">
-        <v>45027</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="3">
+        <v>45027</v>
+      </c>
+      <c r="G4" s="3">
         <v>45024</v>
       </c>
     </row>
@@ -608,17 +605,17 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="3">
         <v>45027</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="7">
-        <v>45027</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="3">
+        <v>45027</v>
+      </c>
+      <c r="E5" s="3">
         <v>45026</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="3">
         <v>45027</v>
       </c>
       <c r="G5" s="1"/>
@@ -627,17 +624,17 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="3">
         <v>45027</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="7">
-        <v>45027</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="3">
+        <v>45027</v>
+      </c>
+      <c r="E6" s="3">
         <v>45026</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="3">
         <v>45027</v>
       </c>
       <c r="G6" s="1"/>
@@ -646,17 +643,17 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7">
-        <v>45027</v>
-      </c>
-      <c r="C7" s="7">
-        <v>45027</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="B7" s="3">
+        <v>45027</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45027</v>
+      </c>
+      <c r="D7" s="3">
         <v>45027</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>45027</v>
       </c>
       <c r="G7" s="1"/>
@@ -665,17 +662,17 @@
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="3">
         <v>45041</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="3">
         <v>45039</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="3">
         <v>45041</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="7">
+      <c r="F8" s="3">
         <v>45041</v>
       </c>
       <c r="G8" s="1"/>
@@ -684,17 +681,17 @@
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="3">
         <v>45048</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="3">
         <v>45047</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="3">
         <v>45048</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="7">
+      <c r="F9" s="3">
         <v>45048</v>
       </c>
       <c r="G9" s="1"/>
@@ -703,17 +700,17 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="3">
         <v>45056</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="3">
         <v>45055</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="3">
         <v>45056</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="7">
+      <c r="F10" s="3">
         <v>45056</v>
       </c>
       <c r="G10" s="1"/>
@@ -722,56 +719,56 @@
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="6">
         <v>45060</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="6">
         <v>45063</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="6">
         <v>45063</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10">
+      <c r="E11" s="7"/>
+      <c r="F11" s="6">
         <v>45063</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="8">
         <v>45063</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="8">
         <v>45063</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="8">
         <v>45063</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="12">
+      <c r="E12" s="9"/>
+      <c r="F12" s="8">
         <v>45063</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="10">
         <v>45070</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14">
+      <c r="C13" s="11"/>
+      <c r="D13" s="10">
         <v>45070</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="14">
+      <c r="E13" s="4"/>
+      <c r="F13" s="10">
         <v>45070</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="10">
         <v>45070</v>
       </c>
     </row>
@@ -779,17 +776,17 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="3">
         <v>45070</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="3">
         <v>45070</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="3">
         <v>45070</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="7">
+      <c r="F14" s="3">
         <v>45070</v>
       </c>
       <c r="G14" s="1"/>
@@ -798,44 +795,50 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="3">
         <v>45077</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="3">
         <v>45077</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="3">
         <v>45077</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="7">
+      <c r="F15" s="3">
         <v>45077</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="7">
-        <v>45023</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="7">
-        <v>45023</v>
+      <c r="B16" s="3">
+        <v>45081</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45081</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45081</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="7">
-        <v>45023</v>
+      <c r="F16" s="3">
+        <v>45081</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45091</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45091</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>

</xml_diff>